<commit_message>
adding groups to test cases
</commit_message>
<xml_diff>
--- a/testdata/Permissions.xlsx
+++ b/testdata/Permissions.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="MCU" sheetId="1" r:id="rId2"/>
+    <sheet name="ASA" sheetId="3" r:id="rId3"/>
+    <sheet name="IT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -89,10 +91,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -111,20 +113,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -133,8 +121,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,16 +168,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -174,6 +193,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -181,33 +208,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,21 +230,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -241,13 +237,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -276,181 +278,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,11 +466,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,45 +544,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -564,148 +566,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -718,52 +720,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1036,8 +1038,8 @@
   <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -1104,8 +1106,8 @@
   <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="$A6:$XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1216,4 +1218,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>